<commit_message>
Realiza Análisis de Ejercicios
</commit_message>
<xml_diff>
--- a/Guia_2/Proyecto_ETL_GA181935/Ejercicio3.xlsx
+++ b/Guia_2/Proyecto_ETL_GA181935/Ejercicio3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garay\Documents\UDB\Ingenieria\2020\Ciclo2\DMD\Laboratorio\Proyecto_ETL_GA181935\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garay\Documents\UDB\Ingenieria\2020\Ciclo2\DMD\Laboratorio\DMD104-01L\Guia_2\Proyecto_ETL_GA181935\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135CE78A-83DB-4E8E-9B61-2B57AABC12AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8817C2D7-A76B-4AEB-9642-1C4C759592C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0EC43B50-8D49-4801-8E3F-CA6E0B41C699}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>CODIGO EMPLEADO</t>
   </si>
@@ -53,6 +53,30 @@
     <t>VENTAS</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1294587-6</t>
+  </si>
+  <si>
+    <t>7894120652-147</t>
+  </si>
+  <si>
+    <t>Maria Leticia</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>9658745-7</t>
+  </si>
+  <si>
+    <t>3658090976-145</t>
+  </si>
+  <si>
+    <t>Christian Alberto</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -65,79 +89,28 @@
     <t>Hernandez Ramirez</t>
   </si>
   <si>
-    <t>Carlos_x000D_
-Roberto</t>
-  </si>
-  <si>
-    <t>750.00</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1294587-6</t>
-  </si>
-  <si>
-    <t>7894120652-147</t>
-  </si>
-  <si>
-    <t>Perez_x000D_
-Hernandez</t>
-  </si>
-  <si>
-    <t>Maria Leticia</t>
-  </si>
-  <si>
-    <t>758.25</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>9658745-7</t>
-  </si>
-  <si>
-    <t>3658090976-145</t>
-  </si>
-  <si>
-    <t>Rodriguez_x000D_
-Arias</t>
-  </si>
-  <si>
-    <t>Christian Alberto</t>
-  </si>
-  <si>
-    <t>857.50</t>
-  </si>
-  <si>
-    <t>Hernandez_x000D_
-Ramirez</t>
-  </si>
-  <si>
     <t>Carlos Roberto</t>
   </si>
   <si>
-    <t>950.00</t>
-  </si>
-  <si>
     <t>Perez Hernandez</t>
   </si>
   <si>
-    <t>Maria_x000D_
-Leticia</t>
-  </si>
-  <si>
-    <t>958.25</t>
-  </si>
-  <si>
     <t>Rodriguez Arias</t>
   </si>
   <si>
-    <t>Christian_x000D_
-Alberto</t>
-  </si>
-  <si>
-    <t>1057.50</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6985847-8</t>
+  </si>
+  <si>
+    <t>4758121280-193</t>
+  </si>
+  <si>
+    <t>Pastori</t>
+  </si>
+  <si>
+    <t>2713.20</t>
   </si>
   <si>
     <t>3</t>
@@ -152,30 +125,22 @@
     <t>Carranza</t>
   </si>
   <si>
-    <t>Pablo_x000D_
-Jose</t>
-  </si>
-  <si>
-    <t>1900.40</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6985847-8</t>
-  </si>
-  <si>
-    <t>4758121280-193</t>
-  </si>
-  <si>
-    <t>Pastori</t>
-  </si>
-  <si>
-    <t>Xavier_x000D_
-Iñaki</t>
-  </si>
-  <si>
-    <t>1912.80</t>
+    <t>2900.60</t>
+  </si>
+  <si>
+    <t>1825.00</t>
+  </si>
+  <si>
+    <t>2216.75</t>
+  </si>
+  <si>
+    <t>2415.50</t>
+  </si>
+  <si>
+    <t>Xavier Iñaki</t>
+  </si>
+  <si>
+    <t>Pablo Jose</t>
   </si>
 </sst>
 </file>
@@ -247,13 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -568,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16123DD0-054F-4EEB-B26B-F021AE15F562}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,164 +566,104 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>